<commit_message>
Updated data from dining services
</commit_message>
<xml_diff>
--- a/Raw Data Seminar Paper/Compost Tracker 3.0.xlsx
+++ b/Raw Data Seminar Paper/Compost Tracker 3.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\My Drive\Courses\ECO324\ECO324 (20_S)\student_help\kate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssayre\Documents\activeProjectRepositories\eco324grading\seminar-paper\seminar-paper-kginder\Raw Data Seminar Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7096611F-A2AC-415B-B8FA-203FEA3DCACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12682410-7669-4D96-B29F-A3A1589726C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="15960" windowHeight="18072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Compost Feb &amp; April" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="15">
   <si>
     <t>Compost Feb &amp; April</t>
   </si>
@@ -1422,21 +1422,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3:F87"/>
+      <selection pane="bottomRight" activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="5" width="16.33203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="17.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="16.33203125" style="1"/>
+    <col min="1" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.6" customHeight="1">
@@ -1607,8 +1607,8 @@
       <c r="F8" s="9">
         <v>25.25</v>
       </c>
-      <c r="G8" s="10">
-        <v>5</v>
+      <c r="G8" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1631,7 +1631,7 @@
         <v>22.5</v>
       </c>
       <c r="G9" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1654,7 +1654,7 @@
         <v>57.75</v>
       </c>
       <c r="G10" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1677,7 +1677,7 @@
         <v>53.5</v>
       </c>
       <c r="G11" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1700,7 +1700,7 @@
         <v>51.25</v>
       </c>
       <c r="G12" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1722,8 +1722,8 @@
       <c r="F13" s="9">
         <v>47.5</v>
       </c>
-      <c r="G13" s="10">
-        <v>10</v>
+      <c r="G13" s="6">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1746,7 +1746,7 @@
         <v>46.5</v>
       </c>
       <c r="G14" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1769,7 +1769,7 @@
         <v>26</v>
       </c>
       <c r="G15" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1792,7 +1792,7 @@
         <v>17.25</v>
       </c>
       <c r="G16" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1815,7 +1815,7 @@
         <v>37.75</v>
       </c>
       <c r="G17" s="10">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1837,8 +1837,8 @@
       <c r="F18" s="9">
         <v>41</v>
       </c>
-      <c r="G18" s="10">
-        <v>15</v>
+      <c r="G18" s="6">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1861,7 +1861,7 @@
         <v>46.25</v>
       </c>
       <c r="G19" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1884,7 +1884,7 @@
         <v>55.25</v>
       </c>
       <c r="G20" s="10">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1907,7 +1907,7 @@
         <v>47.5</v>
       </c>
       <c r="G21" s="10">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1930,7 +1930,7 @@
         <v>30.25</v>
       </c>
       <c r="G22" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1952,8 +1952,8 @@
       <c r="F23" s="9">
         <v>17.5</v>
       </c>
-      <c r="G23" s="10">
-        <v>20</v>
+      <c r="G23" s="6">
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1976,7 +1976,7 @@
         <v>37</v>
       </c>
       <c r="G24" s="10">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -1999,7 +1999,7 @@
         <v>52.75</v>
       </c>
       <c r="G25" s="10">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2022,7 +2022,7 @@
         <v>39.5</v>
       </c>
       <c r="G26" s="10">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2045,7 +2045,7 @@
         <v>57.25</v>
       </c>
       <c r="G27" s="10">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2067,8 +2067,8 @@
       <c r="F28" s="9">
         <v>55.5</v>
       </c>
-      <c r="G28" s="10">
-        <v>25</v>
+      <c r="G28" s="6">
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2091,7 +2091,7 @@
         <v>23</v>
       </c>
       <c r="G29" s="10">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2114,7 +2114,7 @@
         <v>23</v>
       </c>
       <c r="G30" s="10">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2137,7 +2137,7 @@
         <v>29.25</v>
       </c>
       <c r="G31" s="10">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2160,7 +2160,7 @@
         <v>49.25</v>
       </c>
       <c r="G32" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2183,7 +2183,7 @@
         <v>61.75</v>
       </c>
       <c r="G33" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2206,7 +2206,7 @@
         <v>48</v>
       </c>
       <c r="G34" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2229,7 +2229,7 @@
         <v>41.5</v>
       </c>
       <c r="G35" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2252,7 +2252,7 @@
         <v>28.25</v>
       </c>
       <c r="G36" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2275,7 +2275,7 @@
         <v>20.75</v>
       </c>
       <c r="G37" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2298,7 +2298,7 @@
         <v>36.75</v>
       </c>
       <c r="G38" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2321,7 +2321,7 @@
         <v>61.75</v>
       </c>
       <c r="G39" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2344,7 +2344,7 @@
         <v>67</v>
       </c>
       <c r="G40" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2367,7 +2367,7 @@
         <v>56.25</v>
       </c>
       <c r="G41" s="10">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2390,7 +2390,7 @@
         <v>56</v>
       </c>
       <c r="G42" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2413,7 +2413,7 @@
         <v>27.75</v>
       </c>
       <c r="G43" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2436,7 +2436,7 @@
         <v>20.25</v>
       </c>
       <c r="G44" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2459,7 +2459,7 @@
         <v>37</v>
       </c>
       <c r="G45" s="10">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2482,7 +2482,7 @@
         <v>42.5</v>
       </c>
       <c r="G46" s="10">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2505,7 +2505,7 @@
         <v>78.75</v>
       </c>
       <c r="G47" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2528,7 +2528,7 @@
         <v>52.75</v>
       </c>
       <c r="G48" s="10">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2551,7 +2551,7 @@
         <v>39.75</v>
       </c>
       <c r="G49" s="10">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2574,7 +2574,7 @@
         <v>23.5</v>
       </c>
       <c r="G50" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2597,7 +2597,7 @@
         <v>22.25</v>
       </c>
       <c r="G51" s="10">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2620,7 +2620,7 @@
         <v>40.5</v>
       </c>
       <c r="G52" s="10">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2643,7 +2643,7 @@
         <v>54</v>
       </c>
       <c r="G53" s="10">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2666,7 +2666,7 @@
         <v>36.75</v>
       </c>
       <c r="G54" s="10">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2689,7 +2689,7 @@
         <v>43.5</v>
       </c>
       <c r="G55" s="10">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2712,7 +2712,7 @@
         <v>64.75</v>
       </c>
       <c r="G56" s="10">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2735,7 +2735,7 @@
         <v>35.5</v>
       </c>
       <c r="G57" s="10">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2758,7 +2758,7 @@
         <v>18</v>
       </c>
       <c r="G58" s="10">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2781,7 +2781,7 @@
         <v>49.25</v>
       </c>
       <c r="G59" s="10">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2804,7 +2804,7 @@
         <v>53.5</v>
       </c>
       <c r="G60" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2827,7 +2827,7 @@
         <v>57.25</v>
       </c>
       <c r="G61" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2850,7 +2850,7 @@
         <v>53.5</v>
       </c>
       <c r="G62" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2873,7 +2873,7 @@
         <v>45.5</v>
       </c>
       <c r="G63" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2896,7 +2896,7 @@
         <v>27.75</v>
       </c>
       <c r="G64" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2919,7 +2919,7 @@
         <v>23</v>
       </c>
       <c r="G65" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2942,7 +2942,7 @@
         <v>37.75</v>
       </c>
       <c r="G66" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2965,7 +2965,7 @@
         <v>56</v>
       </c>
       <c r="G67" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -2988,7 +2988,7 @@
         <v>47</v>
       </c>
       <c r="G68" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3011,7 +3011,7 @@
         <v>52.75</v>
       </c>
       <c r="G69" s="10">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3034,7 +3034,7 @@
         <v>49.25</v>
       </c>
       <c r="G70" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3057,7 +3057,7 @@
         <v>38.25</v>
       </c>
       <c r="G71" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3080,7 +3080,7 @@
         <v>21.75</v>
       </c>
       <c r="G72" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3103,7 +3103,7 @@
         <v>35.75</v>
       </c>
       <c r="G73" s="10">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3126,7 +3126,7 @@
         <v>57.25</v>
       </c>
       <c r="G74" s="10">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3149,7 +3149,7 @@
         <v>59.75</v>
       </c>
       <c r="G75" s="10">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3172,7 +3172,7 @@
         <v>40.5</v>
       </c>
       <c r="G76" s="10">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3195,7 +3195,7 @@
         <v>56</v>
       </c>
       <c r="G77" s="10">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3218,7 +3218,7 @@
         <v>30.75</v>
       </c>
       <c r="G78" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3241,7 +3241,7 @@
         <v>23.25</v>
       </c>
       <c r="G79" s="10">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3264,7 +3264,7 @@
         <v>51.5</v>
       </c>
       <c r="G80" s="10">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="20.100000000000001" customHeight="1">
@@ -3287,10 +3287,10 @@
         <v>58.5</v>
       </c>
       <c r="G81" s="10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="19.95" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="19.899999999999999" customHeight="1">
       <c r="A82" s="7">
         <v>43949</v>
       </c>
@@ -3310,10 +3310,10 @@
         <v>39.5</v>
       </c>
       <c r="G82" s="10">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="19.95" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="19.899999999999999" customHeight="1">
       <c r="A83" s="7">
         <v>43950</v>
       </c>
@@ -3333,10 +3333,10 @@
         <v>51</v>
       </c>
       <c r="G83" s="10">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="19.95" customHeight="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="19.899999999999999" customHeight="1">
       <c r="A84" s="7">
         <v>43951</v>
       </c>
@@ -3356,10 +3356,10 @@
         <v>48.5</v>
       </c>
       <c r="G84" s="10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="19.95" customHeight="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="19.899999999999999" customHeight="1">
       <c r="A85" s="7">
         <v>43952</v>
       </c>
@@ -3379,10 +3379,10 @@
         <v>34.75</v>
       </c>
       <c r="G85" s="10">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="19.95" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="19.899999999999999" customHeight="1">
       <c r="A86" s="7">
         <v>43953</v>
       </c>
@@ -3402,29 +3402,6 @@
         <v>22.75</v>
       </c>
       <c r="G86" s="10">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A87" s="7">
-        <v>43954</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="9">
-        <v>277</v>
-      </c>
-      <c r="D87" s="5">
-        <v>34.5</v>
-      </c>
-      <c r="E87" s="5">
-        <v>271</v>
-      </c>
-      <c r="F87" s="9">
-        <v>39.5</v>
-      </c>
-      <c r="G87" s="10">
         <v>28</v>
       </c>
     </row>

</xml_diff>